<commit_message>
Updated the error codes to 9xxxx series.
</commit_message>
<xml_diff>
--- a/Error-codes.xlsx
+++ b/Error-codes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Coding\ONDC\ONDC-SRV-Specifications\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD6AF4B-BD0E-4D4F-894C-D39AB2C92C82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C81A51-66E6-4435-A956-FEAE3048166A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -629,7 +629,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -646,9 +646,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1121,8 +1118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93405F62-E538-4EAC-8717-0B01DC84D721}">
   <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82:A97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2273,7 +2270,7 @@
     </row>
     <row r="82" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A82" s="6">
-        <v>70001</v>
+        <v>90004</v>
       </c>
       <c r="B82" s="6" t="s">
         <v>121</v>
@@ -2287,7 +2284,7 @@
     </row>
     <row r="83" spans="1:4" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A83" s="6">
-        <v>71001</v>
+        <v>90005</v>
       </c>
       <c r="B83" s="6" t="s">
         <v>123</v>
@@ -2301,7 +2298,7 @@
     </row>
     <row r="84" spans="1:4" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A84" s="7">
-        <v>71002</v>
+        <v>90006</v>
       </c>
       <c r="B84" s="8" t="s">
         <v>123</v>
@@ -2314,36 +2311,36 @@
       </c>
     </row>
     <row r="85" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A85" s="9">
-        <v>70002</v>
-      </c>
-      <c r="B85" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="C85" s="11" t="s">
+      <c r="A85" s="6">
+        <v>90007</v>
+      </c>
+      <c r="B85" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C85" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="D85" s="11" t="s">
+      <c r="D85" s="10" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A86" s="9">
-        <v>71003</v>
-      </c>
-      <c r="B86" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="C86" s="11" t="s">
+      <c r="A86" s="6">
+        <v>90008</v>
+      </c>
+      <c r="B86" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C86" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="D86" s="11" t="s">
+      <c r="D86" s="10" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A87" s="7">
-        <v>70003</v>
+        <v>90009</v>
       </c>
       <c r="B87" s="8" t="s">
         <v>123</v>
@@ -2356,8 +2353,8 @@
       </c>
     </row>
     <row r="88" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A88" s="7">
-        <v>70004</v>
+      <c r="A88" s="6">
+        <v>90010</v>
       </c>
       <c r="B88" s="8" t="s">
         <v>123</v>
@@ -2370,8 +2367,8 @@
       </c>
     </row>
     <row r="89" spans="1:4" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A89" s="7">
-        <v>70005</v>
+      <c r="A89" s="6">
+        <v>90011</v>
       </c>
       <c r="B89" s="8" t="s">
         <v>123</v>
@@ -2385,7 +2382,7 @@
     </row>
     <row r="90" spans="1:4" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A90" s="7">
-        <v>70006</v>
+        <v>90012</v>
       </c>
       <c r="B90" s="8" t="s">
         <v>123</v>
@@ -2398,10 +2395,10 @@
       </c>
     </row>
     <row r="91" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A91" s="7">
-        <v>71004</v>
-      </c>
-      <c r="B91" s="13" t="s">
+      <c r="A91" s="6">
+        <v>90013</v>
+      </c>
+      <c r="B91" s="12" t="s">
         <v>121</v>
       </c>
       <c r="C91" s="6" t="s">
@@ -2412,10 +2409,10 @@
       </c>
     </row>
     <row r="92" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A92" s="7">
-        <v>71005</v>
-      </c>
-      <c r="B92" s="13" t="s">
+      <c r="A92" s="6">
+        <v>90014</v>
+      </c>
+      <c r="B92" s="12" t="s">
         <v>121</v>
       </c>
       <c r="C92" s="6" t="s">
@@ -2427,9 +2424,9 @@
     </row>
     <row r="93" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A93" s="7">
-        <v>71006</v>
-      </c>
-      <c r="B93" s="13" t="s">
+        <v>90015</v>
+      </c>
+      <c r="B93" s="12" t="s">
         <v>121</v>
       </c>
       <c r="C93" s="6" t="s">
@@ -2441,9 +2438,9 @@
     </row>
     <row r="94" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A94" s="6">
-        <v>71007</v>
-      </c>
-      <c r="B94" s="13" t="s">
+        <v>90016</v>
+      </c>
+      <c r="B94" s="12" t="s">
         <v>121</v>
       </c>
       <c r="C94" s="6" t="s">
@@ -2455,9 +2452,9 @@
     </row>
     <row r="95" spans="1:4" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A95" s="6">
-        <v>71008</v>
-      </c>
-      <c r="B95" s="13" t="s">
+        <v>90017</v>
+      </c>
+      <c r="B95" s="12" t="s">
         <v>121</v>
       </c>
       <c r="C95" s="6" t="s">
@@ -2468,10 +2465,10 @@
       </c>
     </row>
     <row r="96" spans="1:4" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A96" s="6">
-        <v>71009</v>
-      </c>
-      <c r="B96" s="13" t="s">
+      <c r="A96" s="7">
+        <v>90018</v>
+      </c>
+      <c r="B96" s="12" t="s">
         <v>121</v>
       </c>
       <c r="C96" s="6" t="s">
@@ -2483,9 +2480,9 @@
     </row>
     <row r="97" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A97" s="6">
-        <v>71010</v>
-      </c>
-      <c r="B97" s="13" t="s">
+        <v>90019</v>
+      </c>
+      <c r="B97" s="12" t="s">
         <v>121</v>
       </c>
       <c r="C97" s="6" t="s">

</xml_diff>